<commit_message>
fixing auth bug, update time table
</commit_message>
<xml_diff>
--- a/register/out.xlsx
+++ b/register/out.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="MySheet" state="show" r:id="rId4"/>
+    <sheet name="MySheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="357">
   <si>
     <t>Name</t>
   </si>
@@ -770,19 +773,331 @@
   </si>
   <si>
     <t>L0561</t>
+  </si>
+  <si>
+    <t>กัลยาณี โนจิตร</t>
+  </si>
+  <si>
+    <t>ครีม</t>
+  </si>
+  <si>
+    <t>0613163215</t>
+  </si>
+  <si>
+    <t>M0562</t>
+  </si>
+  <si>
+    <t>รัตนวดี ศรีมา</t>
+  </si>
+  <si>
+    <t>หลิว</t>
+  </si>
+  <si>
+    <t>0830822669</t>
+  </si>
+  <si>
+    <t>L0563</t>
+  </si>
+  <si>
+    <t>อัครภา หล้าต๋า</t>
+  </si>
+  <si>
+    <t>อีฟ</t>
+  </si>
+  <si>
+    <t>0882582302</t>
+  </si>
+  <si>
+    <t>M0564</t>
+  </si>
+  <si>
+    <t>วิชฌาญา ประดุงสิทธิ์</t>
+  </si>
+  <si>
+    <t>ฟาร์</t>
+  </si>
+  <si>
+    <t>0648833414</t>
+  </si>
+  <si>
+    <t>L0665</t>
+  </si>
+  <si>
+    <t>พรภวิกา หมั่นฝึกพันธ์</t>
+  </si>
+  <si>
+    <t>แบมแบม</t>
+  </si>
+  <si>
+    <t>0957031637</t>
+  </si>
+  <si>
+    <t>M0666</t>
+  </si>
+  <si>
+    <t>ภควดี บุญปกครอง</t>
+  </si>
+  <si>
+    <t>แคท</t>
+  </si>
+  <si>
+    <t>0888718594</t>
+  </si>
+  <si>
+    <t>M0567</t>
+  </si>
+  <si>
+    <t>ปพัชญา สมบัติเจริญกิจ</t>
+  </si>
+  <si>
+    <t>มัดหมี่</t>
+  </si>
+  <si>
+    <t>0932799339</t>
+  </si>
+  <si>
+    <t>M0468</t>
+  </si>
+  <si>
+    <t>มัชฌมน รินนาศักดิ์</t>
+  </si>
+  <si>
+    <t>ลูกตาล</t>
+  </si>
+  <si>
+    <t>0988645849</t>
+  </si>
+  <si>
+    <t>M0569</t>
+  </si>
+  <si>
+    <t>อริสา มิมาละ</t>
+  </si>
+  <si>
+    <t>ยิม</t>
+  </si>
+  <si>
+    <t>0946037334</t>
+  </si>
+  <si>
+    <t>L0570</t>
+  </si>
+  <si>
+    <t>พุดน้ำบุษย์ จำรัส</t>
+  </si>
+  <si>
+    <t>นาน่า</t>
+  </si>
+  <si>
+    <t>0823837299</t>
+  </si>
+  <si>
+    <t>L0571</t>
+  </si>
+  <si>
+    <t>รัฐพล ไชยอิ่นคำ</t>
+  </si>
+  <si>
+    <t>หมีพูห์</t>
+  </si>
+  <si>
+    <t>0990830472</t>
+  </si>
+  <si>
+    <t>M0572</t>
+  </si>
+  <si>
+    <t>วุฒิชัย ทาป้อ</t>
+  </si>
+  <si>
+    <t>วุดดี้</t>
+  </si>
+  <si>
+    <t>0979571742</t>
+  </si>
+  <si>
+    <t>L0573</t>
+  </si>
+  <si>
+    <t>ภัสราพร จันเลน</t>
+  </si>
+  <si>
+    <t>สตางค์</t>
+  </si>
+  <si>
+    <t>0932130492</t>
+  </si>
+  <si>
+    <t>M0574</t>
+  </si>
+  <si>
+    <t>นิธิยา คำแก้ว</t>
+  </si>
+  <si>
+    <t>มารูโกะ</t>
+  </si>
+  <si>
+    <t>0908939417</t>
+  </si>
+  <si>
+    <t>L0575</t>
+  </si>
+  <si>
+    <t>กัลยาณี รักฝูง</t>
+  </si>
+  <si>
+    <t>มด</t>
+  </si>
+  <si>
+    <t>0903327945</t>
+  </si>
+  <si>
+    <t>M0576</t>
+  </si>
+  <si>
+    <t>อาซี แซ่จ๋าว</t>
+  </si>
+  <si>
+    <t>อาซี</t>
+  </si>
+  <si>
+    <t>0848547954</t>
+  </si>
+  <si>
+    <t>L0577</t>
+  </si>
+  <si>
+    <t>ฌัชชา ธนะชัยขันธ์</t>
+  </si>
+  <si>
+    <t>เฌอปอ</t>
+  </si>
+  <si>
+    <t>0946352120</t>
+  </si>
+  <si>
+    <t>XL0578</t>
+  </si>
+  <si>
+    <t>สุภนิดา เดชะบุญ</t>
+  </si>
+  <si>
+    <t>หงส์</t>
+  </si>
+  <si>
+    <t>0823858098</t>
+  </si>
+  <si>
+    <t>L0579</t>
+  </si>
+  <si>
+    <t>ฐิติพร มะโนวรรณา</t>
+  </si>
+  <si>
+    <t>ข้าวฟ่าง</t>
+  </si>
+  <si>
+    <t>0843687160</t>
+  </si>
+  <si>
+    <t>M0580</t>
+  </si>
+  <si>
+    <t>กวิสรา ต๊ะหล้า</t>
+  </si>
+  <si>
+    <t>ใบเตย</t>
+  </si>
+  <si>
+    <t>0987806334</t>
+  </si>
+  <si>
+    <t>M0581</t>
+  </si>
+  <si>
+    <t>นภสร พิทักษ์กำพล</t>
+  </si>
+  <si>
+    <t>หมอก</t>
+  </si>
+  <si>
+    <t>0956875377</t>
+  </si>
+  <si>
+    <t>L0582</t>
+  </si>
+  <si>
+    <t>พิมพ์วิไล ชัยปัน</t>
+  </si>
+  <si>
+    <t>ใบเต0ย</t>
+  </si>
+  <si>
+    <t>0991036153</t>
+  </si>
+  <si>
+    <t>M0583</t>
+  </si>
+  <si>
+    <t>พชรพร พรมนิกร</t>
+  </si>
+  <si>
+    <t>มี่</t>
+  </si>
+  <si>
+    <t>0642859039</t>
+  </si>
+  <si>
+    <t>M0584</t>
+  </si>
+  <si>
+    <t>ธันยธรณ์ แก้วมีศรี</t>
+  </si>
+  <si>
+    <t>รวงข้าว</t>
+  </si>
+  <si>
+    <t>0611456944</t>
+  </si>
+  <si>
+    <t>M0685</t>
+  </si>
+  <si>
+    <t>ธนพรพรรณ ม่วงเจริญ</t>
+  </si>
+  <si>
+    <t>ออม</t>
+  </si>
+  <si>
+    <t>0936206845</t>
+  </si>
+  <si>
+    <t>M0486</t>
+  </si>
+  <si>
+    <t>นิภากร ผัสวี</t>
+  </si>
+  <si>
+    <t>เฟิร์ส</t>
+  </si>
+  <si>
+    <t>0958026853</t>
+  </si>
+  <si>
+    <t>M0587</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -805,8 +1120,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1146,8 +1462,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F62"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <dimension ref="A1:F88"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2339,7 +2664,7 @@
       <c r="C60" t="s">
         <v>8</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="1">
         <v>1234567890</v>
       </c>
       <c r="E60" t="s">
@@ -2389,8 +2714,528 @@
         <v>252</v>
       </c>
     </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>253</v>
+      </c>
+      <c r="B63" t="s">
+        <v>254</v>
+      </c>
+      <c r="C63" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" t="s">
+        <v>255</v>
+      </c>
+      <c r="E63" t="s">
+        <v>10</v>
+      </c>
+      <c r="F63" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>257</v>
+      </c>
+      <c r="B64" t="s">
+        <v>258</v>
+      </c>
+      <c r="C64" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" t="s">
+        <v>259</v>
+      </c>
+      <c r="E64" t="s">
+        <v>15</v>
+      </c>
+      <c r="F64" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>261</v>
+      </c>
+      <c r="B65" t="s">
+        <v>262</v>
+      </c>
+      <c r="C65" t="s">
+        <v>8</v>
+      </c>
+      <c r="D65" t="s">
+        <v>263</v>
+      </c>
+      <c r="E65" t="s">
+        <v>10</v>
+      </c>
+      <c r="F65" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>265</v>
+      </c>
+      <c r="B66" t="s">
+        <v>266</v>
+      </c>
+      <c r="C66" t="s">
+        <v>19</v>
+      </c>
+      <c r="D66" t="s">
+        <v>267</v>
+      </c>
+      <c r="E66" t="s">
+        <v>15</v>
+      </c>
+      <c r="F66" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>269</v>
+      </c>
+      <c r="B67" t="s">
+        <v>270</v>
+      </c>
+      <c r="C67" t="s">
+        <v>19</v>
+      </c>
+      <c r="D67" t="s">
+        <v>271</v>
+      </c>
+      <c r="E67" t="s">
+        <v>10</v>
+      </c>
+      <c r="F67" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>273</v>
+      </c>
+      <c r="B68" t="s">
+        <v>274</v>
+      </c>
+      <c r="C68" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" t="s">
+        <v>275</v>
+      </c>
+      <c r="E68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F68" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>277</v>
+      </c>
+      <c r="B69" t="s">
+        <v>278</v>
+      </c>
+      <c r="C69" t="s">
+        <v>36</v>
+      </c>
+      <c r="D69" t="s">
+        <v>279</v>
+      </c>
+      <c r="E69" t="s">
+        <v>10</v>
+      </c>
+      <c r="F69" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>281</v>
+      </c>
+      <c r="B70" t="s">
+        <v>282</v>
+      </c>
+      <c r="C70" t="s">
+        <v>8</v>
+      </c>
+      <c r="D70" t="s">
+        <v>283</v>
+      </c>
+      <c r="E70" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>285</v>
+      </c>
+      <c r="B71" t="s">
+        <v>286</v>
+      </c>
+      <c r="C71" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" t="s">
+        <v>287</v>
+      </c>
+      <c r="E71" t="s">
+        <v>15</v>
+      </c>
+      <c r="F71" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>289</v>
+      </c>
+      <c r="B72" t="s">
+        <v>290</v>
+      </c>
+      <c r="C72" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" t="s">
+        <v>291</v>
+      </c>
+      <c r="E72" t="s">
+        <v>15</v>
+      </c>
+      <c r="F72" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>293</v>
+      </c>
+      <c r="B73" t="s">
+        <v>294</v>
+      </c>
+      <c r="C73" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" t="s">
+        <v>295</v>
+      </c>
+      <c r="E73" t="s">
+        <v>10</v>
+      </c>
+      <c r="F73" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>297</v>
+      </c>
+      <c r="B74" t="s">
+        <v>298</v>
+      </c>
+      <c r="C74" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" t="s">
+        <v>299</v>
+      </c>
+      <c r="E74" t="s">
+        <v>15</v>
+      </c>
+      <c r="F74" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>301</v>
+      </c>
+      <c r="B75" t="s">
+        <v>302</v>
+      </c>
+      <c r="C75" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" t="s">
+        <v>303</v>
+      </c>
+      <c r="E75" t="s">
+        <v>10</v>
+      </c>
+      <c r="F75" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>305</v>
+      </c>
+      <c r="B76" t="s">
+        <v>306</v>
+      </c>
+      <c r="C76" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" t="s">
+        <v>307</v>
+      </c>
+      <c r="E76" t="s">
+        <v>15</v>
+      </c>
+      <c r="F76" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>309</v>
+      </c>
+      <c r="B77" t="s">
+        <v>310</v>
+      </c>
+      <c r="C77" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" t="s">
+        <v>311</v>
+      </c>
+      <c r="E77" t="s">
+        <v>10</v>
+      </c>
+      <c r="F77" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>313</v>
+      </c>
+      <c r="B78" t="s">
+        <v>314</v>
+      </c>
+      <c r="C78" t="s">
+        <v>8</v>
+      </c>
+      <c r="D78" t="s">
+        <v>315</v>
+      </c>
+      <c r="E78" t="s">
+        <v>15</v>
+      </c>
+      <c r="F78" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>317</v>
+      </c>
+      <c r="B79" t="s">
+        <v>318</v>
+      </c>
+      <c r="C79" t="s">
+        <v>8</v>
+      </c>
+      <c r="D79" t="s">
+        <v>319</v>
+      </c>
+      <c r="E79" t="s">
+        <v>79</v>
+      </c>
+      <c r="F79" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>321</v>
+      </c>
+      <c r="B80" t="s">
+        <v>322</v>
+      </c>
+      <c r="C80" t="s">
+        <v>8</v>
+      </c>
+      <c r="D80" t="s">
+        <v>323</v>
+      </c>
+      <c r="E80" t="s">
+        <v>15</v>
+      </c>
+      <c r="F80" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>325</v>
+      </c>
+      <c r="B81" t="s">
+        <v>326</v>
+      </c>
+      <c r="C81" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" t="s">
+        <v>327</v>
+      </c>
+      <c r="E81" t="s">
+        <v>10</v>
+      </c>
+      <c r="F81" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>329</v>
+      </c>
+      <c r="B82" t="s">
+        <v>330</v>
+      </c>
+      <c r="C82" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" t="s">
+        <v>331</v>
+      </c>
+      <c r="E82" t="s">
+        <v>10</v>
+      </c>
+      <c r="F82" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>333</v>
+      </c>
+      <c r="B83" t="s">
+        <v>334</v>
+      </c>
+      <c r="C83" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" t="s">
+        <v>335</v>
+      </c>
+      <c r="E83" t="s">
+        <v>15</v>
+      </c>
+      <c r="F83" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>337</v>
+      </c>
+      <c r="B84" t="s">
+        <v>338</v>
+      </c>
+      <c r="C84" t="s">
+        <v>8</v>
+      </c>
+      <c r="D84" t="s">
+        <v>339</v>
+      </c>
+      <c r="E84" t="s">
+        <v>10</v>
+      </c>
+      <c r="F84" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>341</v>
+      </c>
+      <c r="B85" t="s">
+        <v>342</v>
+      </c>
+      <c r="C85" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85" t="s">
+        <v>343</v>
+      </c>
+      <c r="E85" t="s">
+        <v>10</v>
+      </c>
+      <c r="F85" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>345</v>
+      </c>
+      <c r="B86" t="s">
+        <v>346</v>
+      </c>
+      <c r="C86" t="s">
+        <v>19</v>
+      </c>
+      <c r="D86" t="s">
+        <v>347</v>
+      </c>
+      <c r="E86" t="s">
+        <v>10</v>
+      </c>
+      <c r="F86" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>349</v>
+      </c>
+      <c r="B87" t="s">
+        <v>350</v>
+      </c>
+      <c r="C87" t="s">
+        <v>36</v>
+      </c>
+      <c r="D87" t="s">
+        <v>351</v>
+      </c>
+      <c r="E87" t="s">
+        <v>10</v>
+      </c>
+      <c r="F87" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>353</v>
+      </c>
+      <c r="B88" t="s">
+        <v>354</v>
+      </c>
+      <c r="C88" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" t="s">
+        <v>355</v>
+      </c>
+      <c r="E88" t="s">
+        <v>10</v>
+      </c>
+      <c r="F88" t="s">
+        <v>356</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>